<commit_message>
Commit: fixed issues in GA
</commit_message>
<xml_diff>
--- a/Student Data.xlsx
+++ b/Student Data.xlsx
@@ -1352,28 +1352,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="21.6484375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="11" width="21.6484375" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="7" width="19.5" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="7" width="21.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="7" width="21.5" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="7" width="23.1484375" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="7" width="21.6484375" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="7" width="21.5" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="7" width="21.34765625" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" style="7" width="21.6484375" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" style="7" width="19.34765625" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" style="7" width="22.1484375" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" style="7" width="21.34765625" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" style="7" width="22.0" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" style="7" width="22.34765625" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" style="7" width="21.34765625" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" style="7" width="21.84765625" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" style="7" width="22.5" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" style="7" width="21.5" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" style="7" width="22.1484375" collapsed="false"/>
-    <col min="23" max="23" customWidth="true" style="7" width="21.84765625" collapsed="false"/>
-    <col min="24" max="24" customWidth="true" style="7" width="21.34765625" collapsed="false"/>
+    <col min="1" max="3" customWidth="true" width="21.6484375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="11" width="21.6484375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="7" width="19.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="7" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="7" width="21.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="7" width="23.1484375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="7" width="21.6484375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="7" width="21.5" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="7" width="21.34765625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="7" width="21.6484375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="7" width="19.34765625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="7" width="22.1484375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="7" width="21.34765625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="7" width="22.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="7" width="22.34765625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="7" width="21.34765625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="7" width="21.84765625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="7" width="22.5" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="7" width="21.5" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="7" width="22.1484375" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="7" width="21.84765625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="7" width="21.34765625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.6">

</xml_diff>